<commit_message>
work on organizatorial notebooks
</commit_message>
<xml_diff>
--- a/projects/Groups-And-Exercise-Classes.xlsx
+++ b/projects/Groups-And-Exercise-Classes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="232">
   <si>
     <t>Group</t>
   </si>
@@ -112,402 +112,405 @@
     <t>group_st</t>
   </si>
   <si>
+    <t>gustav-og-daniel</t>
+  </si>
+  <si>
+    <t>jeppe-hersh-signe</t>
+  </si>
+  <si>
+    <t>jonathan-og-anna</t>
+  </si>
+  <si>
+    <t>lads</t>
+  </si>
+  <si>
+    <t>learning-c</t>
+  </si>
+  <si>
+    <t>lost_in_optimization</t>
+  </si>
+  <si>
+    <t>ludvigsen</t>
+  </si>
+  <si>
+    <t>mads-rasmus-kristian</t>
+  </si>
+  <si>
+    <t>madsholleufer</t>
+  </si>
+  <si>
+    <t>markus-kasper</t>
+  </si>
+  <si>
+    <t>mmf</t>
+  </si>
+  <si>
+    <t>msm</t>
+  </si>
+  <si>
+    <t>my_anaconda_don-t</t>
+  </si>
+  <si>
+    <t>paulaemma-s</t>
+  </si>
+  <si>
+    <t>ppap</t>
+  </si>
+  <si>
+    <t>rasmus-markus</t>
+  </si>
+  <si>
+    <t>rebekka-og-alex</t>
+  </si>
+  <si>
+    <t>rsi-team</t>
+  </si>
+  <si>
+    <t>sabrina-christoffer</t>
+  </si>
+  <si>
+    <t>sadek-som-statsminister</t>
+  </si>
+  <si>
+    <t>scandies</t>
+  </si>
+  <si>
+    <t>simon-nick</t>
+  </si>
+  <si>
+    <t>sophsim</t>
+  </si>
+  <si>
+    <t>sprit-af</t>
+  </si>
+  <si>
+    <t>studentsbreadsarerated</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>team-1</t>
+  </si>
+  <si>
+    <t>team-123</t>
+  </si>
+  <si>
+    <t>team-2</t>
+  </si>
+  <si>
+    <t>team-4-4-2</t>
+  </si>
+  <si>
+    <t>team-abc</t>
+  </si>
+  <si>
+    <t>team-eyu</t>
+  </si>
+  <si>
+    <t>team-freelvlau</t>
+  </si>
+  <si>
+    <t>team-hjn</t>
+  </si>
+  <si>
+    <t>team-team</t>
+  </si>
+  <si>
+    <t>team-weuh</t>
+  </si>
+  <si>
+    <t>teamhackerhannah</t>
+  </si>
+  <si>
+    <t>teamp-up</t>
+  </si>
+  <si>
+    <t>teamtea</t>
+  </si>
+  <si>
+    <t>three-horses</t>
+  </si>
+  <si>
+    <t>torsdag</t>
+  </si>
+  <si>
+    <t>vpn</t>
+  </si>
+  <si>
+    <t>dmz246</t>
+  </si>
+  <si>
+    <t>A5k3r</t>
+  </si>
+  <si>
+    <t>Christine-Bach</t>
+  </si>
+  <si>
+    <t>albertehoeg</t>
+  </si>
+  <si>
+    <t>amandachris97</t>
+  </si>
+  <si>
+    <t>GustavRugaard</t>
+  </si>
+  <si>
+    <t>ansofol</t>
+  </si>
+  <si>
+    <t>JakobMPython</t>
+  </si>
+  <si>
+    <t>annakargo</t>
+  </si>
+  <si>
+    <t>cbh819</t>
+  </si>
+  <si>
+    <t>jxw232</t>
+  </si>
+  <si>
+    <t>AmalieBusk</t>
+  </si>
+  <si>
+    <t>TobiasLynggaardEcon</t>
+  </si>
+  <si>
+    <t>jkt210</t>
+  </si>
+  <si>
+    <t>cecilietut</t>
+  </si>
+  <si>
+    <t>kqb729</t>
+  </si>
+  <si>
+    <t>Gvdwnse</t>
+  </si>
+  <si>
+    <t>jonas-hass-bonne</t>
+  </si>
+  <si>
+    <t>madsrl</t>
+  </si>
+  <si>
+    <t>marcusengholm</t>
+  </si>
+  <si>
+    <t>Nikodrengen3</t>
+  </si>
+  <si>
+    <t>wsn658</t>
+  </si>
+  <si>
+    <t>victorfunch</t>
+  </si>
+  <si>
+    <t>rasmusklitte</t>
+  </si>
+  <si>
+    <t>christiandanpedersen</t>
+  </si>
+  <si>
+    <t>yapicikerem</t>
+  </si>
+  <si>
     <t>guccimane1996</t>
   </si>
   <si>
-    <t>gustav-og-daniel</t>
-  </si>
-  <si>
-    <t>jeppe-hersh-signe</t>
-  </si>
-  <si>
-    <t>jonathan-og-anna</t>
-  </si>
-  <si>
-    <t>lads</t>
-  </si>
-  <si>
-    <t>learning-c</t>
-  </si>
-  <si>
-    <t>lost_in_optimization</t>
-  </si>
-  <si>
-    <t>ludvigsen</t>
-  </si>
-  <si>
-    <t>mads-rasmus-kristian</t>
-  </si>
-  <si>
-    <t>madsholleufer</t>
-  </si>
-  <si>
-    <t>marko_og_david</t>
-  </si>
-  <si>
-    <t>markus-kasper</t>
-  </si>
-  <si>
-    <t>mmf</t>
-  </si>
-  <si>
-    <t>msm</t>
-  </si>
-  <si>
-    <t>my_anaconda_don-t</t>
-  </si>
-  <si>
-    <t>paulaemma-s</t>
-  </si>
-  <si>
-    <t>ppap</t>
-  </si>
-  <si>
-    <t>rasmus-markus</t>
-  </si>
-  <si>
-    <t>rebekka-og-alex</t>
-  </si>
-  <si>
-    <t>rsi-team</t>
-  </si>
-  <si>
-    <t>sabrina-christoffer</t>
-  </si>
-  <si>
-    <t>sadek-som-statsminister</t>
-  </si>
-  <si>
-    <t>scandies</t>
-  </si>
-  <si>
-    <t>simon-nick</t>
-  </si>
-  <si>
-    <t>sophsim</t>
-  </si>
-  <si>
-    <t>sprit-af</t>
-  </si>
-  <si>
-    <t>studentsbreadsarerated</t>
-  </si>
-  <si>
-    <t>team</t>
-  </si>
-  <si>
-    <t>team-1</t>
-  </si>
-  <si>
-    <t>team-123</t>
-  </si>
-  <si>
-    <t>team-2</t>
-  </si>
-  <si>
-    <t>team-4-4-2</t>
-  </si>
-  <si>
-    <t>team-abc</t>
-  </si>
-  <si>
-    <t>team-eyu</t>
-  </si>
-  <si>
-    <t>team-freelvlau</t>
-  </si>
-  <si>
-    <t>team-hjn</t>
-  </si>
-  <si>
-    <t>team-team</t>
-  </si>
-  <si>
-    <t>teamhackerhannah</t>
-  </si>
-  <si>
-    <t>teamp-up</t>
-  </si>
-  <si>
-    <t>teamtea</t>
-  </si>
-  <si>
-    <t>three-horses</t>
-  </si>
-  <si>
-    <t>torsdag</t>
-  </si>
-  <si>
-    <t>vpn</t>
+    <t>Dencker123</t>
+  </si>
+  <si>
+    <t>Sxc757</t>
+  </si>
+  <si>
+    <t>annalangelund</t>
+  </si>
+  <si>
+    <t>ptd207</t>
+  </si>
+  <si>
+    <t>Alexh1988</t>
+  </si>
+  <si>
+    <t>pythonslayer</t>
+  </si>
+  <si>
+    <t>RasmusLudvigsen</t>
+  </si>
+  <si>
+    <t>KristianLundqvistKragelund</t>
+  </si>
+  <si>
+    <t>markusrask</t>
+  </si>
+  <si>
+    <t>LarsenFred</t>
+  </si>
+  <si>
+    <t>Stulli20</t>
+  </si>
+  <si>
+    <t>Jakob385</t>
+  </si>
+  <si>
+    <t>EmmaaaLange</t>
+  </si>
+  <si>
+    <t>nicolaipeytz</t>
+  </si>
+  <si>
+    <t>markusekstrom</t>
+  </si>
+  <si>
+    <t>nxv593</t>
+  </si>
+  <si>
+    <t>is232022</t>
+  </si>
+  <si>
+    <t>ChrisPaivinen</t>
+  </si>
+  <si>
+    <t>sade0024</t>
+  </si>
+  <si>
+    <t>caroblom</t>
+  </si>
+  <si>
+    <t>NickDahl91</t>
+  </si>
+  <si>
+    <t>Ismondur</t>
+  </si>
+  <si>
+    <t>Bernseng</t>
+  </si>
+  <si>
+    <t>TheoRaaTho</t>
+  </si>
+  <si>
+    <t>Matiboy1998</t>
+  </si>
+  <si>
+    <t>pkrogsager</t>
+  </si>
+  <si>
+    <t>Ganganguinga</t>
+  </si>
+  <si>
+    <t>StineDittmann</t>
+  </si>
+  <si>
+    <t>LasseStrand</t>
+  </si>
+  <si>
+    <t>djt951</t>
+  </si>
+  <si>
+    <t>ureichenberg</t>
+  </si>
+  <si>
+    <t>frejakatharina</t>
+  </si>
+  <si>
+    <t>henrietta345</t>
+  </si>
+  <si>
+    <t>jensknudsen</t>
   </si>
   <si>
     <t>ankaer</t>
   </si>
   <si>
-    <t>A5k3r</t>
-  </si>
-  <si>
-    <t>Christine-Bach</t>
-  </si>
-  <si>
-    <t>albertehoeg</t>
-  </si>
-  <si>
-    <t>amandachris97</t>
-  </si>
-  <si>
-    <t>GustavRugaard</t>
-  </si>
-  <si>
-    <t>ansofol</t>
-  </si>
-  <si>
-    <t>JakobMPython</t>
-  </si>
-  <si>
-    <t>annakargo</t>
-  </si>
-  <si>
-    <t>cbh819</t>
-  </si>
-  <si>
-    <t>jxw232</t>
-  </si>
-  <si>
-    <t>AmalieBusk</t>
-  </si>
-  <si>
-    <t>TobiasLynggaardEcon</t>
-  </si>
-  <si>
-    <t>jkt210</t>
-  </si>
-  <si>
-    <t>cecilietut</t>
-  </si>
-  <si>
-    <t>kqb729</t>
-  </si>
-  <si>
-    <t>Gvdwnse</t>
-  </si>
-  <si>
-    <t>jonas-hass-bonne</t>
-  </si>
-  <si>
-    <t>madsrl</t>
-  </si>
-  <si>
-    <t>marcusengholm</t>
-  </si>
-  <si>
-    <t>Nikodrengen3</t>
-  </si>
-  <si>
-    <t>wsn658</t>
-  </si>
-  <si>
-    <t>victorfunch</t>
-  </si>
-  <si>
-    <t>rasmusklitte</t>
-  </si>
-  <si>
-    <t>christiandanpedersen</t>
-  </si>
-  <si>
-    <t>yapicikerem</t>
-  </si>
-  <si>
-    <t>jhumasheikh</t>
-  </si>
-  <si>
-    <t>Dencker123</t>
-  </si>
-  <si>
-    <t>Sxc757</t>
-  </si>
-  <si>
-    <t>annalangelund</t>
+    <t>tps798</t>
+  </si>
+  <si>
+    <t>AdamFJ97</t>
+  </si>
+  <si>
+    <t>KU-TeamT</t>
+  </si>
+  <si>
+    <t>Asbjornjp</t>
+  </si>
+  <si>
+    <t>KamilPan</t>
+  </si>
+  <si>
+    <t>cwv570</t>
+  </si>
+  <si>
+    <t>dmx963</t>
+  </si>
+  <si>
+    <t>kasperloewer</t>
+  </si>
+  <si>
+    <t>czq776</t>
+  </si>
+  <si>
+    <t>qcn966</t>
+  </si>
+  <si>
+    <t>Anacondainstaller</t>
+  </si>
+  <si>
+    <t>AnnaBlanpied</t>
+  </si>
+  <si>
+    <t>olivernystrom</t>
+  </si>
+  <si>
+    <t>crd852</t>
+  </si>
+  <si>
+    <t>nxz636</t>
+  </si>
+  <si>
+    <t>ClaraRashid</t>
+  </si>
+  <si>
+    <t>ghz106</t>
+  </si>
+  <si>
+    <t>TuePoulsen</t>
+  </si>
+  <si>
+    <t>zohlen</t>
+  </si>
+  <si>
+    <t>MJKibsgaard</t>
+  </si>
+  <si>
+    <t>VincentRDahl</t>
+  </si>
+  <si>
+    <t>JacobClausen99</t>
+  </si>
+  <si>
+    <t>ditjj</t>
+  </si>
+  <si>
+    <t>Kasperjaco99</t>
+  </si>
+  <si>
+    <t>Nielsla</t>
+  </si>
+  <si>
+    <t>tsf643</t>
+  </si>
+  <si>
+    <t>rjk323</t>
+  </si>
+  <si>
+    <t>fjk508</t>
   </si>
   <si>
     <t>AnthonElm2</t>
   </si>
   <si>
-    <t>Alexh1988</t>
-  </si>
-  <si>
-    <t>pythonslayer</t>
-  </si>
-  <si>
-    <t>RasmusLudvigsen</t>
-  </si>
-  <si>
-    <t>KristianLundqvistKragelund</t>
-  </si>
-  <si>
-    <t>Ganganguinga</t>
-  </si>
-  <si>
-    <t>markusrask</t>
-  </si>
-  <si>
-    <t>LarsenFred</t>
-  </si>
-  <si>
-    <t>Stulli20</t>
-  </si>
-  <si>
-    <t>Jakob385</t>
-  </si>
-  <si>
-    <t>EmmaaaLange</t>
-  </si>
-  <si>
-    <t>nicolaipeytz</t>
-  </si>
-  <si>
-    <t>markusekstrom</t>
-  </si>
-  <si>
-    <t>nxv593</t>
-  </si>
-  <si>
-    <t>is232022</t>
-  </si>
-  <si>
-    <t>ChrisPaivinen</t>
-  </si>
-  <si>
-    <t>sade0024</t>
-  </si>
-  <si>
-    <t>caroblom</t>
-  </si>
-  <si>
-    <t>NickDahl91</t>
-  </si>
-  <si>
-    <t>Ismondur</t>
-  </si>
-  <si>
-    <t>Bernseng</t>
-  </si>
-  <si>
-    <t>TheoRaaTho</t>
-  </si>
-  <si>
-    <t>Matiboy1998</t>
-  </si>
-  <si>
-    <t>pkrogsager</t>
-  </si>
-  <si>
-    <t>StineDittmann</t>
-  </si>
-  <si>
-    <t>LasseStrand</t>
-  </si>
-  <si>
-    <t>djt951</t>
-  </si>
-  <si>
-    <t>ureichenberg</t>
-  </si>
-  <si>
-    <t>frejakatharina</t>
-  </si>
-  <si>
-    <t>henrietta345</t>
-  </si>
-  <si>
-    <t>jensknudsen</t>
-  </si>
-  <si>
-    <t>tps798</t>
-  </si>
-  <si>
-    <t>AdamFJ97</t>
-  </si>
-  <si>
-    <t>KU-TeamT</t>
-  </si>
-  <si>
-    <t>Asbjornjp</t>
-  </si>
-  <si>
-    <t>KamilPan</t>
-  </si>
-  <si>
-    <t>cwv570</t>
-  </si>
-  <si>
-    <t>dmz246</t>
-  </si>
-  <si>
-    <t>kasperloewer</t>
-  </si>
-  <si>
-    <t>czq776</t>
-  </si>
-  <si>
-    <t>qcn966</t>
-  </si>
-  <si>
-    <t>Anacondainstaller</t>
-  </si>
-  <si>
-    <t>AnnaBlanpied</t>
-  </si>
-  <si>
-    <t>olivernystrom</t>
-  </si>
-  <si>
-    <t>crd852</t>
-  </si>
-  <si>
-    <t>nxz636</t>
-  </si>
-  <si>
-    <t>ClaraRashid</t>
-  </si>
-  <si>
-    <t>ghz106</t>
-  </si>
-  <si>
-    <t>TuePoulsen</t>
-  </si>
-  <si>
-    <t>zohlen</t>
-  </si>
-  <si>
-    <t>MJKibsgaard</t>
-  </si>
-  <si>
-    <t>VincentRDahl</t>
-  </si>
-  <si>
-    <t>JacobClausen99</t>
-  </si>
-  <si>
-    <t>ditjj</t>
-  </si>
-  <si>
-    <t>Kasperjaco99</t>
-  </si>
-  <si>
-    <t>Nielsla</t>
-  </si>
-  <si>
-    <t>tsf643</t>
-  </si>
-  <si>
-    <t>rjk323</t>
-  </si>
-  <si>
-    <t>fjk508</t>
-  </si>
-  <si>
     <t>nikbipbip</t>
   </si>
   <si>
@@ -517,60 +520,60 @@
     <t>nbz937</t>
   </si>
   <si>
+    <t>Kranker97</t>
+  </si>
+  <si>
+    <t>mfgunnesmo</t>
+  </si>
+  <si>
+    <t>Vibaek96</t>
+  </si>
+  <si>
+    <t>Danielle974</t>
+  </si>
+  <si>
+    <t>emmaebrl</t>
+  </si>
+  <si>
+    <t>WilfulUrchin58</t>
+  </si>
+  <si>
+    <t>MDonsJ</t>
+  </si>
+  <si>
+    <t>RebekkaJoensen</t>
+  </si>
+  <si>
+    <t>gbl667</t>
+  </si>
+  <si>
+    <t>hsr522git</t>
+  </si>
+  <si>
+    <t>andersborstrom</t>
+  </si>
+  <si>
+    <t>huludev</t>
+  </si>
+  <si>
+    <t>Fitzdyhr</t>
+  </si>
+  <si>
+    <t>SophieSteiness</t>
+  </si>
+  <si>
+    <t>elen0281</t>
+  </si>
+  <si>
+    <t>JonaDelaney</t>
+  </si>
+  <si>
+    <t>PeterBCarlsen</t>
+  </si>
+  <si>
     <t>DavidReynisson</t>
   </si>
   <si>
-    <t>Kranker97</t>
-  </si>
-  <si>
-    <t>mfgunnesmo</t>
-  </si>
-  <si>
-    <t>Vibaek96</t>
-  </si>
-  <si>
-    <t>Danielle974</t>
-  </si>
-  <si>
-    <t>emmaebrl</t>
-  </si>
-  <si>
-    <t>WilfulUrchin58</t>
-  </si>
-  <si>
-    <t>MDonsJ</t>
-  </si>
-  <si>
-    <t>RebekkaJoensen</t>
-  </si>
-  <si>
-    <t>gbl667</t>
-  </si>
-  <si>
-    <t>hsr522git</t>
-  </si>
-  <si>
-    <t>andersborstrom</t>
-  </si>
-  <si>
-    <t>huludev</t>
-  </si>
-  <si>
-    <t>Fitzdyhr</t>
-  </si>
-  <si>
-    <t>SophieSteiness</t>
-  </si>
-  <si>
-    <t>elen0281</t>
-  </si>
-  <si>
-    <t>JonaDelaney</t>
-  </si>
-  <si>
-    <t>PeterBCarlsen</t>
-  </si>
-  <si>
     <t>Astridlw</t>
   </si>
   <si>
@@ -607,9 +610,6 @@
     <t>PetrosChristoforou</t>
   </si>
   <si>
-    <t>dmx963</t>
-  </si>
-  <si>
     <t>KarlMagnusHovmand</t>
   </si>
   <si>
@@ -644,6 +644,9 @@
   </si>
   <si>
     <t>SigneALT</t>
+  </si>
+  <si>
+    <t>Storstormand</t>
   </si>
   <si>
     <t>rzf875</t>
@@ -1064,7 +1067,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1092,13 +1095,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
         <v>142</v>
-      </c>
-      <c r="D2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1106,7 +1106,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1114,7 +1114,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
         <v>143</v>
@@ -1125,7 +1125,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
         <v>144</v>
@@ -1136,7 +1136,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
         <v>145</v>
@@ -1147,7 +1147,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1155,7 +1155,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1163,7 +1163,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
         <v>146</v>
@@ -1177,7 +1177,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1185,7 +1185,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
         <v>147</v>
@@ -1199,7 +1199,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1207,7 +1207,7 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1215,7 +1215,7 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" t="s">
         <v>148</v>
@@ -1229,7 +1229,7 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
         <v>149</v>
@@ -1240,7 +1240,7 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" t="s">
         <v>150</v>
@@ -1254,7 +1254,7 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
         <v>151</v>
@@ -1265,7 +1265,7 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
         <v>152</v>
@@ -1276,7 +1276,7 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1284,7 +1284,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
         <v>153</v>
@@ -1298,7 +1298,7 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
         <v>154</v>
@@ -1312,7 +1312,7 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
         <v>155</v>
@@ -1326,7 +1326,7 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
         <v>156</v>
@@ -1340,7 +1340,7 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C24" t="s">
         <v>157</v>
@@ -1354,7 +1354,7 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
         <v>158</v>
@@ -1368,7 +1368,7 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" t="s">
         <v>159</v>
@@ -1382,7 +1382,7 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" t="s">
         <v>160</v>
@@ -1393,7 +1393,7 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1403,6 +1403,9 @@
       <c r="B29" t="s">
         <v>101</v>
       </c>
+      <c r="C29" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
@@ -1412,7 +1415,10 @@
         <v>102</v>
       </c>
       <c r="C30" t="s">
-        <v>161</v>
+        <v>162</v>
+      </c>
+      <c r="D30" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1423,10 +1429,7 @@
         <v>103</v>
       </c>
       <c r="C31" t="s">
-        <v>162</v>
-      </c>
-      <c r="D31" t="s">
-        <v>209</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1437,7 +1440,10 @@
         <v>104</v>
       </c>
       <c r="C32" t="s">
-        <v>163</v>
+        <v>164</v>
+      </c>
+      <c r="D32" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1447,6 +1453,9 @@
       <c r="B33" t="s">
         <v>105</v>
       </c>
+      <c r="C33" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
@@ -1456,7 +1465,10 @@
         <v>106</v>
       </c>
       <c r="C34" t="s">
-        <v>164</v>
+        <v>166</v>
+      </c>
+      <c r="D34" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1466,12 +1478,6 @@
       <c r="B35" t="s">
         <v>107</v>
       </c>
-      <c r="C35" t="s">
-        <v>165</v>
-      </c>
-      <c r="D35" t="s">
-        <v>210</v>
-      </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
@@ -1480,19 +1486,19 @@
       <c r="B36" t="s">
         <v>108</v>
       </c>
+      <c r="C36" t="s">
+        <v>167</v>
+      </c>
+      <c r="D36" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>109</v>
-      </c>
-      <c r="C37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D37" t="s">
-        <v>211</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1500,7 +1506,10 @@
         <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>109</v>
+      </c>
+      <c r="C38" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1511,7 +1520,10 @@
         <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>167</v>
+        <v>169</v>
+      </c>
+      <c r="D39" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1522,7 +1534,10 @@
         <v>111</v>
       </c>
       <c r="C40" t="s">
-        <v>168</v>
+        <v>170</v>
+      </c>
+      <c r="D40" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1533,10 +1548,10 @@
         <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D41" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1547,10 +1562,10 @@
         <v>113</v>
       </c>
       <c r="C42" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D42" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1561,10 +1576,10 @@
         <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D43" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1575,10 +1590,10 @@
         <v>115</v>
       </c>
       <c r="C44" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D44" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1589,10 +1604,7 @@
         <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>173</v>
-      </c>
-      <c r="D45" t="s">
-        <v>216</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1603,10 +1615,10 @@
         <v>117</v>
       </c>
       <c r="C46" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D46" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1617,7 +1629,7 @@
         <v>118</v>
       </c>
       <c r="C47" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1628,10 +1640,10 @@
         <v>119</v>
       </c>
       <c r="C48" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D48" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1642,7 +1654,7 @@
         <v>120</v>
       </c>
       <c r="C49" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1653,10 +1665,7 @@
         <v>121</v>
       </c>
       <c r="C50" t="s">
-        <v>178</v>
-      </c>
-      <c r="D50" t="s">
-        <v>219</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1667,7 +1676,7 @@
         <v>122</v>
       </c>
       <c r="C51" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1678,7 +1687,7 @@
         <v>123</v>
       </c>
       <c r="C52" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1689,7 +1698,7 @@
         <v>124</v>
       </c>
       <c r="C53" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1700,7 +1709,7 @@
         <v>125</v>
       </c>
       <c r="C54" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1710,9 +1719,6 @@
       <c r="B55" t="s">
         <v>126</v>
       </c>
-      <c r="C55" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
@@ -1722,7 +1728,10 @@
         <v>127</v>
       </c>
       <c r="C56" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="D56" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1732,19 +1741,22 @@
       <c r="B57" t="s">
         <v>128</v>
       </c>
+      <c r="C57" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="C58" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="D58" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1752,10 +1764,13 @@
         <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C59" t="s">
-        <v>185</v>
+        <v>188</v>
+      </c>
+      <c r="D59" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1763,13 +1778,13 @@
         <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C60" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D60" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1777,13 +1792,13 @@
         <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C61" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D61" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1791,13 +1806,13 @@
         <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C62" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D62" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1805,13 +1820,13 @@
         <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C63" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D63" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1819,13 +1834,10 @@
         <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C64" t="s">
-        <v>190</v>
-      </c>
-      <c r="D64" t="s">
-        <v>225</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1833,13 +1845,10 @@
         <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C65" t="s">
-        <v>191</v>
-      </c>
-      <c r="D65" t="s">
-        <v>226</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1847,10 +1856,13 @@
         <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C66" t="s">
-        <v>192</v>
+        <v>194</v>
+      </c>
+      <c r="D66" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1858,13 +1870,7 @@
         <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>137</v>
-      </c>
-      <c r="C67" t="s">
-        <v>193</v>
-      </c>
-      <c r="D67" t="s">
-        <v>227</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1872,7 +1878,13 @@
         <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>138</v>
+        <v>139</v>
+      </c>
+      <c r="C68" t="s">
+        <v>195</v>
+      </c>
+      <c r="D68" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1880,13 +1892,13 @@
         <v>72</v>
       </c>
       <c r="B69" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C69" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D69" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1894,27 +1906,13 @@
         <v>73</v>
       </c>
       <c r="B70" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C70" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D70" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" t="s">
-        <v>74</v>
-      </c>
-      <c r="B71" t="s">
-        <v>141</v>
-      </c>
-      <c r="C71" t="s">
-        <v>196</v>
-      </c>
-      <c r="D71" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>